<commit_message>
Adding more results and changes on README
</commit_message>
<xml_diff>
--- a/datasets/hetrec2011-lastfm-2k/results_path[policy=last_items=005_reorder=10_hybrid].xlsx
+++ b/datasets/hetrec2011-lastfm-2k/results_path[policy=last_items=005_reorder=10_hybrid].xlsx
@@ -8,6 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="bprmf" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="mostpop" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="wikidata_page_rank8020" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ease" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="userknn" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ncf" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1053,4 +1058,2836 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>METRIC</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED MEAN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE NAME</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE MEAN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>WILCOXON</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TTEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MAP@1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.09498999999999999</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.07055630000000002</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.11969228774605e-05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MAP@3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1305933</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.09896369999999999</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.976492996484947e-11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MAP@5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1367643</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1061771</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5.668489791573369e-12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAP@10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1384439</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1099716</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.461745482477754e-12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AGG_DIV@1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>16</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.948580292960369e-08</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AGG_DIV@3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5.572586364565697e-09</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AGG_DIV@5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.5134306016405e-07</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NDCG@1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.09498999999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.07055630000000002</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.11969228774605e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NDCG@3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.1648657</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1261181</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7.414496067093443e-07</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NDCG@5</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1785318</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1417091</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.689107927314242e-09</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NDCG@10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.187302</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1599637</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5.604385718640215e-09</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>GINI@1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9994016990472702</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.9997026646503665</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8.3956370803474e-13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GINI@3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.9991114952672074</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9994437711859074</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3.307419710861618e-14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GINI@5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9989246643502068</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9992092470076116</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.502953277924573e-13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ENTROPY@1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8477123827114259</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.4094788897618311</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.597937545606194e-12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ENTROPY@3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1.055102529782206</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.8012843040331677</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6.651066589217021e-16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ENTROPY@5</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1.144846957772855</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.9798600769807638</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.637651705576595e-14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>COVERAGE@1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.001447636528561131</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0008323486477198104</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3.03158790370231e-08</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>COVERAGE@3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.002162354283190432</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.00136620774169588</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5.374056980359882e-09</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COVERAGE@5</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.002424720689633548</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.001890916562514423</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>mostpop</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.500061678819395e-07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>METRIC</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED MEAN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE NAME</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE MEAN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>WILCOXON</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TTEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MAP@1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1767085</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.155034</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.347926672809036e-08</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MAP@3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2231781</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1989087</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3.156304491978218e-09</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MAP@5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.2308839</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2077577</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.186370040878349e-08</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAP@10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2294772</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2097982</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.300410328606449e-08</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AGG_DIV@1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>106.8</v>
+      </c>
+      <c r="D6" t="n">
+        <v>60.5</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.520580786161087e-09</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AGG_DIV@3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>201.8</v>
+      </c>
+      <c r="D7" t="n">
+        <v>125.1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.035202747033812e-11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AGG_DIV@5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>247</v>
+      </c>
+      <c r="D8" t="n">
+        <v>179.7</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4.847859052481416e-09</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NDCG@1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1767085</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.155034</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.347926672809036e-08</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NDCG@3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.267522</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.2410809</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.258699698806114e-08</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NDCG@5</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.2865212</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.2615261</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.963209345529895e-08</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NDCG@10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.297719</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.2807471</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.10990337594672e-08</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>GINI@1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9983371873136679</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.999148078418673</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4.609371713712576e-12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GINI@3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.9975816550491841</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9985797404579054</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.118635392621496e-13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GINI@5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9972848382070156</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9980992475632288</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.163029019593483e-12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ENTROPY@1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1.296031398685581</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.9659338376329168</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2.130027728861465e-16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ENTROPY@3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1.480027575213429</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.248093708734896</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G17" t="n">
+        <v>9.442446504366149e-16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ENTROPY@5</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1.547063633207895</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.394584524861939</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.932941523019162e-15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>COVERAGE@1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.009663215486358796</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.005474060357277087</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.524780297365677e-09</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>COVERAGE@3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.01825863875904363</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01131872613049094</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2.210911838815081e-11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COVERAGE@5</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.02234846183257841</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.01625922558564188</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>wikidata_page_rank8020</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4.899309167039847e-09</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>METRIC</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED MEAN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE NAME</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE MEAN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>WILCOXON</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TTEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MAP@1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.239461</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2406582000000001</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.431640625</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.4485070762789973</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MAP@3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2999084</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2987568</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.3931618571970348</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MAP@5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.309328</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3089521</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6953125</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.7304956904471269</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAP@10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3028609</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.3033393</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.556640625</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.5544793524465665</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AGG_DIV@1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>173.6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.032197353070125e-08</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AGG_DIV@3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>336.6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>266.6</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5.250947828455492e-11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AGG_DIV@5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>444.7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>375.4</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.389431932067418e-10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NDCG@1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.239461</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2406582000000001</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.431640625</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.4485070762789973</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NDCG@3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.3582782</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.354578</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.037109375</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.04822606868773735</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NDCG@5</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3817144</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.3807355</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.431640625</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.3451214115990352</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NDCG@10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.3963081000000001</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.3964652000000001</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.8528989332054997</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>GINI@1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9958129226074464</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.9967700981024793</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8.368632710790571e-10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GINI@3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.9933701064143499</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9946510292288895</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5.802983140721409e-12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GINI@5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9917530772883097</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9930031201724911</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.252458586662432e-12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ENTROPY@1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1.7447912039351</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.639263592805119</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4.603112959196203e-10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ENTROPY@3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1.950375006180462</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.869539750314361</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.037430470085653e-11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ENTROPY@5</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2.051311085644614</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.989784942033803</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.188283176579372e-12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>COVERAGE@1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.01570707733458661</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01201567816744792</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.030216417115009e-08</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>COVERAGE@3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.03045472961422435</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.02412160711629055</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4.989059140686237e-11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COVERAGE@5</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.04023484013117215</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.03396462948577187</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ease</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2.493401878106313e-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>METRIC</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED MEAN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE NAME</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE MEAN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>WILCOXON</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TTEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MAP@1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.2209897</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2252162</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.037109375</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.04743748038327212</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MAP@3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2824019</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2846711</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.10546875</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1107581263718558</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MAP@5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.2923142</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2942325</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.083984375</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1891552593082108</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAP@10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2875579</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2903418999999999</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.037109375</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.02668187747132254</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AGG_DIV@1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>195.9</v>
+      </c>
+      <c r="D6" t="n">
+        <v>155.5</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.388373110536241e-08</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AGG_DIV@3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>372.3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>294.6</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.961732883780602e-11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AGG_DIV@5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>477.7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>400</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.370166419028014e-09</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NDCG@1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.2209897</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2252162</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.037109375</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.04743748038327212</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NDCG@3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.3410427</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.3412182</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.76953125</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9274258074605891</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NDCG@5</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3655521</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.365383</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.845703125</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9096744860491095</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>NDCG@10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.3807948</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.3821086</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.2037849462971191</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>GINI@1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9948950054920479</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.995950728911408</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5.634916103853265e-10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GINI@3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.9921614324734953</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.9936924021804184</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3.324835126406628e-12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GINI@5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9903655674689945</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9918566007939488</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2.023193689099743e-11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ENTROPY@1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1.831167702701879</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.73899533647183</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2.790716779746172e-09</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ENTROPY@3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2.019073991657447</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.93924536292086</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.704025196300161e-12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ENTROPY@5</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2.114341407293851</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.05306564510915</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.277975214418885e-11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>COVERAGE@1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0177246715392254</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01406952543721147</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.371944395514816e-08</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>COVERAGE@3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.03368419592176505</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0266546318381675</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.756248373148618e-11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COVERAGE@5</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.04321992079005975</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.03619061871394352</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>userknn</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.280947176764666e-09</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>METRIC</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PROPOSED MEAN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE NAME</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BASELINE MEAN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>WILCOXON</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TTEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MAP@1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1786024</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.167172</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.665371392927721e-05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MAP@3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2459271</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2350459999999999</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.248841043289412e-06</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MAP@5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.2633357</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2543502999999999</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.26992516127065e-06</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAP@10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.278034</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2695313</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.808441099167078e-06</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NDCG@1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1786024</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.167172</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.665371392927721e-05</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NDCG@3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3111002</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.300625</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8.761805895227904e-06</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NDCG@5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.3469481</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.3404047</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.549969347386081e-05</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NDCG@10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>path[policy=last_items=005_reorder=10_hybrid]</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.3851863</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3793497</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ncf</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.001953125</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5.357732332481631e-06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>